<commit_message>
genauigkeit auch bei \d\d.\d einem, new records
</commit_message>
<xml_diff>
--- a/WPMTracker/WPM.xlsx
+++ b/WPMTracker/WPM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\WPMTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D6CA89-23F0-4E2B-8250-A5F4BCB8DBAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05D0507-EC19-41F8-9FC5-869422778096}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2490" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Nr.</t>
   </si>
@@ -90,6 +90,9 @@
   <si>
     <t>97.47</t>
   </si>
+  <si>
+    <t>95.9</t>
+  </si>
 </sst>
 </file>
 
@@ -98,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +150,19 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,8 +277,44 @@
         <bgColor rgb="FFDD5151"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FF9BC2E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FFA9D08E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD5151"/>
+        <bgColor rgb="FFDD5151"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -329,11 +379,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -411,6 +472,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="21" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -696,7 +778,7 @@
   <dimension ref="A1:I4434"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,8 +1230,33 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
-      <c r="G16" s="1"/>
+      <c r="A16" s="27">
+        <v>15</v>
+      </c>
+      <c r="B16" s="28">
+        <v>44312.485564768518</v>
+      </c>
+      <c r="C16" s="29">
+        <v>103</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="31">
+        <v>536</v>
+      </c>
+      <c r="F16" s="32">
+        <v>515</v>
+      </c>
+      <c r="G16" s="33">
+        <v>21</v>
+      </c>
+      <c r="H16" s="32">
+        <v>96</v>
+      </c>
+      <c r="I16" s="33">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>

</xml_diff>

<commit_message>
aufgeräumt und graph überarbeitet
</commit_message>
<xml_diff>
--- a/WPMTracker/WPM.xlsx
+++ b/WPMTracker/WPM.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="2490" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="WPM" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WPM" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1568,7 +1568,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="42" t="n">
-        <v>44312.67528114574</v>
+        <v>44312.67528114584</v>
       </c>
       <c r="C21" s="43" t="n">
         <v>99</v>
@@ -1595,16 +1595,97 @@
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="12" t="n"/>
-      <c r="G22" s="1" t="n"/>
+      <c r="A22" s="41" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="42" t="n">
+        <v>44313.48644244213</v>
+      </c>
+      <c r="C22" s="43" t="n">
+        <v>92</v>
+      </c>
+      <c r="D22" s="44" t="inlineStr">
+        <is>
+          <t>89.51</t>
+        </is>
+      </c>
+      <c r="E22" s="45" t="n">
+        <v>509</v>
+      </c>
+      <c r="F22" s="46" t="n">
+        <v>461</v>
+      </c>
+      <c r="G22" s="47" t="n">
+        <v>48</v>
+      </c>
+      <c r="H22" s="46" t="n">
+        <v>81</v>
+      </c>
+      <c r="I22" s="47" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="23">
-      <c r="B23" s="12" t="n"/>
-      <c r="G23" s="1" t="n"/>
+      <c r="A23" s="41" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="42" t="n">
+        <v>44313.71834622685</v>
+      </c>
+      <c r="C23" s="43" t="n">
+        <v>87</v>
+      </c>
+      <c r="D23" s="44" t="inlineStr">
+        <is>
+          <t>94.37</t>
+        </is>
+      </c>
+      <c r="E23" s="45" t="n">
+        <v>446</v>
+      </c>
+      <c r="F23" s="46" t="n">
+        <v>436</v>
+      </c>
+      <c r="G23" s="47" t="n">
+        <v>10</v>
+      </c>
+      <c r="H23" s="46" t="n">
+        <v>83</v>
+      </c>
+      <c r="I23" s="47" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
-      <c r="B24" s="12" t="n"/>
-      <c r="G24" s="1" t="n"/>
+      <c r="A24" s="41" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="42" t="n">
+        <v>44313.76618999836</v>
+      </c>
+      <c r="C24" s="43" t="n">
+        <v>91</v>
+      </c>
+      <c r="D24" s="44" t="inlineStr">
+        <is>
+          <t>92.64</t>
+        </is>
+      </c>
+      <c r="E24" s="45" t="n">
+        <v>484</v>
+      </c>
+      <c r="F24" s="46" t="n">
+        <v>453</v>
+      </c>
+      <c r="G24" s="47" t="n">
+        <v>31</v>
+      </c>
+      <c r="H24" s="46" t="n">
+        <v>86</v>
+      </c>
+      <c r="I24" s="47" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="12" t="n"/>

</xml_diff>